<commit_message>
Refactor user information update logic and API endpoint
</commit_message>
<xml_diff>
--- a/upload/小程序用户信息导入模板.xlsx
+++ b/upload/小程序用户信息导入模板.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15410" windowHeight="5910"/>
+    <workbookView windowWidth="19200" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>姓名</t>
   </si>
@@ -50,15 +50,6 @@
   </si>
   <si>
     <t>积分（佣金）</t>
-  </si>
-  <si>
-    <t>张梅</t>
-  </si>
-  <si>
-    <t>山西省</t>
-  </si>
-  <si>
-    <t>太原市</t>
   </si>
 </sst>
 </file>
@@ -704,23 +695,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1036,16 +1027,16 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="2" width="12.7272727272727" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.4545454545455" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.1818181818182" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.6363636363636" style="2" customWidth="1"/>
-    <col min="6" max="6" width="16" style="2" customWidth="1"/>
+    <col min="3" max="3" width="14.4545454545455" customWidth="1"/>
+    <col min="4" max="4" width="21.1818181818182" customWidth="1"/>
+    <col min="5" max="5" width="17.6363636363636" customWidth="1"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="21.3636363636364" customWidth="1"/>
     <col min="8" max="8" width="17.3636363636364" customWidth="1"/>
     <col min="9" max="9" width="15.1818181818182" customWidth="1"/>
@@ -1054,7 +1045,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1063,47 +1054,35 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="G1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="6">
-        <v>15903417788</v>
-      </c>
-      <c r="E2" s="6">
-        <v>2</v>
-      </c>
-      <c r="F2" s="6">
-        <v>80</v>
-      </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="5"/>
@@ -1112,11 +1091,11 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="5"/>
@@ -1125,11 +1104,11 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="5"/>
@@ -1138,11 +1117,11 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="5"/>
@@ -1151,11 +1130,11 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="5"/>
@@ -1164,11 +1143,11 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="5"/>
@@ -1177,11 +1156,11 @@
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="5"/>
@@ -1190,11 +1169,11 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5"/>
@@ -1203,11 +1182,11 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5"/>
@@ -1216,11 +1195,11 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="5"/>
@@ -1229,11 +1208,11 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="5"/>
@@ -1242,11 +1221,11 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="5"/>
@@ -1255,11 +1234,11 @@
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="5"/>
@@ -1268,11 +1247,11 @@
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="5"/>
@@ -1281,11 +1260,11 @@
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="5"/>
@@ -1294,11 +1273,11 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="5"/>
@@ -1307,11 +1286,11 @@
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="5"/>
@@ -1320,11 +1299,11 @@
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5"/>
@@ -1333,11 +1312,11 @@
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="5"/>
@@ -1346,11 +1325,11 @@
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="5"/>
@@ -1359,11 +1338,11 @@
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>